<commit_message>
Discovered that MLP learns much better
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/max_prefix_clip_grad_1_step_3e_4_no_norm/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/max_prefix_clip_grad_1_step_3e_4_no_norm/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3276"/>
+  <dimension ref="A1:C3279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43020,6 +43020,45 @@
         <v>13.99455305375514</v>
       </c>
     </row>
+    <row r="3277">
+      <c r="A3277" s="1" t="n">
+        <v>3275</v>
+      </c>
+      <c r="B3277" t="inlineStr">
+        <is>
+          <t>[6, -6, -4]</t>
+        </is>
+      </c>
+      <c r="C3277" t="n">
+        <v>14.00913491406147</v>
+      </c>
+    </row>
+    <row r="3278">
+      <c r="A3278" s="1" t="n">
+        <v>3276</v>
+      </c>
+      <c r="B3278" t="inlineStr">
+        <is>
+          <t>[7, -5, 1]</t>
+        </is>
+      </c>
+      <c r="C3278" t="n">
+        <v>14.57563135050274</v>
+      </c>
+    </row>
+    <row r="3279">
+      <c r="A3279" s="1" t="n">
+        <v>3277</v>
+      </c>
+      <c r="B3279" t="inlineStr">
+        <is>
+          <t>[7, -2, -5]</t>
+        </is>
+      </c>
+      <c r="C3279" t="n">
+        <v>14.08510830351622</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>